<commit_message>
Trained Keras CNN on Vids 1-6 dataset including fillers. Accuracy dropped from 71% to 64%
</commit_message>
<xml_diff>
--- a/Classifications/Cleaned/Classifications_Vids123_filled.xlsx
+++ b/Classifications/Cleaned/Classifications_Vids123_filled.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aha_mp3/SSTP/aerobictextreviewLFS/Classifications/Cleaning/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aha_mp3/SSTP/aerobictextreviewLFS/Classifications/Cleaned/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A516681-7CCE-654B-B3F8-A3EB0C4BE9D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C7162EE-966D-4846-8DD6-61DCF20396FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10660" yWindow="1740" windowWidth="31560" windowHeight="24460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25000" yWindow="1740" windowWidth="17220" windowHeight="24460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1658" uniqueCount="838">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1662" uniqueCount="840">
   <si>
     <t>familiarExercisePhrases</t>
   </si>
@@ -1502,12 +1502,6 @@
     <t>big reach</t>
   </si>
   <si>
-    <t>so from the box it's a little easier, standing a little harder</t>
-  </si>
-  <si>
-    <t>standing it forces me to use a little bit more stability and a little bit more core</t>
-  </si>
-  <si>
     <t>this is about that point in the workout where you start to really feel it</t>
   </si>
   <si>
@@ -2552,6 +2546,18 @@
   </si>
   <si>
     <t>when you're here if you feel good or you can just stay here</t>
+  </si>
+  <si>
+    <t>so from the box it's a little easier</t>
+  </si>
+  <si>
+    <t>standing a little harder</t>
+  </si>
+  <si>
+    <t>a little bit more stability</t>
+  </si>
+  <si>
+    <t>a little bit more core</t>
   </si>
 </sst>
 </file>
@@ -3424,10 +3430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E829"/>
+  <dimension ref="A1:E831"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A787" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="C826" sqref="C826"/>
+    <sheetView tabSelected="1" topLeftCell="A762" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="B781" sqref="B781"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3437,7 +3443,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -3445,7 +3451,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -3453,7 +3459,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -3461,7 +3467,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -3477,7 +3483,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="B6" t="s">
         <v>0</v>
@@ -3485,7 +3491,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="B7" t="s">
         <v>0</v>
@@ -3501,7 +3507,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="B9" t="s">
         <v>0</v>
@@ -3597,7 +3603,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="B21" t="s">
         <v>0</v>
@@ -3605,7 +3611,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="B22" t="s">
         <v>0</v>
@@ -3629,7 +3635,7 @@
     </row>
     <row r="25" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="B25" t="s">
         <v>1</v>
@@ -3637,7 +3643,7 @@
     </row>
     <row r="26" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B26" t="s">
         <v>1</v>
@@ -3645,7 +3651,7 @@
     </row>
     <row r="27" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="B27" t="s">
         <v>1</v>
@@ -3703,7 +3709,7 @@
     </row>
     <row r="34" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="B34" t="s">
         <v>1</v>
@@ -3711,7 +3717,7 @@
     </row>
     <row r="35" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="B35" t="s">
         <v>1</v>
@@ -3719,7 +3725,7 @@
     </row>
     <row r="36" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="B36" t="s">
         <v>1</v>
@@ -3727,7 +3733,7 @@
     </row>
     <row r="37" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="B37" t="s">
         <v>1</v>
@@ -3735,7 +3741,7 @@
     </row>
     <row r="38" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B38" t="s">
         <v>1</v>
@@ -3743,7 +3749,7 @@
     </row>
     <row r="39" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B39" t="s">
         <v>1</v>
@@ -3751,7 +3757,7 @@
     </row>
     <row r="40" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="B40" t="s">
         <v>1</v>
@@ -3759,7 +3765,7 @@
     </row>
     <row r="41" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="B41" t="s">
         <v>1</v>
@@ -3799,7 +3805,7 @@
     </row>
     <row r="46" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="B46" t="s">
         <v>1</v>
@@ -3807,7 +3813,7 @@
     </row>
     <row r="47" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="B47" t="s">
         <v>1</v>
@@ -3823,7 +3829,7 @@
     </row>
     <row r="49" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="B49" t="s">
         <v>1</v>
@@ -3831,7 +3837,7 @@
     </row>
     <row r="50" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="B50" t="s">
         <v>1</v>
@@ -3839,7 +3845,7 @@
     </row>
     <row r="51" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="B51" t="s">
         <v>1</v>
@@ -3855,7 +3861,7 @@
     </row>
     <row r="53" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="B53" t="s">
         <v>1</v>
@@ -3863,7 +3869,7 @@
     </row>
     <row r="54" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="B54" t="s">
         <v>1</v>
@@ -3871,7 +3877,7 @@
     </row>
     <row r="55" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="B55" t="s">
         <v>1</v>
@@ -3879,7 +3885,7 @@
     </row>
     <row r="56" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="B56" t="s">
         <v>1</v>
@@ -3887,7 +3893,7 @@
     </row>
     <row r="57" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="B57" t="s">
         <v>1</v>
@@ -3895,7 +3901,7 @@
     </row>
     <row r="58" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B58" t="s">
         <v>1</v>
@@ -3903,7 +3909,7 @@
     </row>
     <row r="59" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="B59" t="s">
         <v>1</v>
@@ -3911,7 +3917,7 @@
     </row>
     <row r="60" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="B60" t="s">
         <v>1</v>
@@ -3919,7 +3925,7 @@
     </row>
     <row r="61" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="B61" t="s">
         <v>1</v>
@@ -3927,7 +3933,7 @@
     </row>
     <row r="62" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="B62" t="s">
         <v>1</v>
@@ -3935,7 +3941,7 @@
     </row>
     <row r="63" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="B63" t="s">
         <v>1</v>
@@ -3943,7 +3949,7 @@
     </row>
     <row r="64" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="B64" t="s">
         <v>1</v>
@@ -3975,7 +3981,7 @@
     </row>
     <row r="68" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="B68" t="s">
         <v>1</v>
@@ -3983,7 +3989,7 @@
     </row>
     <row r="69" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="B69" t="s">
         <v>1</v>
@@ -3991,7 +3997,7 @@
     </row>
     <row r="70" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="B70" t="s">
         <v>1</v>
@@ -3999,7 +4005,7 @@
     </row>
     <row r="71" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="B71" t="s">
         <v>1</v>
@@ -4007,7 +4013,7 @@
     </row>
     <row r="72" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="B72" t="s">
         <v>1</v>
@@ -4015,7 +4021,7 @@
     </row>
     <row r="73" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="B73" t="s">
         <v>1</v>
@@ -4023,7 +4029,7 @@
     </row>
     <row r="74" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="B74" t="s">
         <v>1</v>
@@ -4047,7 +4053,7 @@
     </row>
     <row r="77" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="B77" t="s">
         <v>1</v>
@@ -4063,7 +4069,7 @@
     </row>
     <row r="79" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="B79" t="s">
         <v>1</v>
@@ -4071,7 +4077,7 @@
     </row>
     <row r="80" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="B80" t="s">
         <v>1</v>
@@ -4079,7 +4085,7 @@
     </row>
     <row r="81" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="B81" t="s">
         <v>1</v>
@@ -4095,7 +4101,7 @@
     </row>
     <row r="83" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="B83" t="s">
         <v>1</v>
@@ -4103,7 +4109,7 @@
     </row>
     <row r="84" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="B84" t="s">
         <v>1</v>
@@ -4111,7 +4117,7 @@
     </row>
     <row r="85" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="B85" t="s">
         <v>1</v>
@@ -4119,7 +4125,7 @@
     </row>
     <row r="86" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="B86" t="s">
         <v>1</v>
@@ -4135,7 +4141,7 @@
     </row>
     <row r="88" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="B88" t="s">
         <v>1</v>
@@ -4151,7 +4157,7 @@
     </row>
     <row r="90" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="B90" t="s">
         <v>1</v>
@@ -4159,7 +4165,7 @@
     </row>
     <row r="91" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="B91" t="s">
         <v>1</v>
@@ -4167,7 +4173,7 @@
     </row>
     <row r="92" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="B92" t="s">
         <v>1</v>
@@ -4183,7 +4189,7 @@
     </row>
     <row r="94" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="B94" t="s">
         <v>1</v>
@@ -4191,7 +4197,7 @@
     </row>
     <row r="95" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="B95" t="s">
         <v>1</v>
@@ -4199,7 +4205,7 @@
     </row>
     <row r="96" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="B96" t="s">
         <v>1</v>
@@ -4207,7 +4213,7 @@
     </row>
     <row r="97" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="B97" t="s">
         <v>1</v>
@@ -4215,7 +4221,7 @@
     </row>
     <row r="98" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="B98" t="s">
         <v>1</v>
@@ -4223,7 +4229,7 @@
     </row>
     <row r="99" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="B99" t="s">
         <v>1</v>
@@ -4239,7 +4245,7 @@
     </row>
     <row r="101" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="B101" t="s">
         <v>1</v>
@@ -4263,7 +4269,7 @@
     </row>
     <row r="104" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="B104" t="s">
         <v>1</v>
@@ -4271,7 +4277,7 @@
     </row>
     <row r="105" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="B105" t="s">
         <v>1</v>
@@ -4279,7 +4285,7 @@
     </row>
     <row r="106" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="B106" t="s">
         <v>1</v>
@@ -4287,7 +4293,7 @@
     </row>
     <row r="107" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="B107" t="s">
         <v>1</v>
@@ -4295,7 +4301,7 @@
     </row>
     <row r="108" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="B108" t="s">
         <v>1</v>
@@ -4303,7 +4309,7 @@
     </row>
     <row r="109" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="B109" t="s">
         <v>1</v>
@@ -4327,7 +4333,7 @@
     </row>
     <row r="112" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="B112" t="s">
         <v>1</v>
@@ -4335,7 +4341,7 @@
     </row>
     <row r="113" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="B113" t="s">
         <v>1</v>
@@ -4343,7 +4349,7 @@
     </row>
     <row r="114" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="B114" t="s">
         <v>1</v>
@@ -4359,7 +4365,7 @@
     </row>
     <row r="116" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="B116" t="s">
         <v>1</v>
@@ -4367,7 +4373,7 @@
     </row>
     <row r="117" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="B117" t="s">
         <v>1</v>
@@ -4383,7 +4389,7 @@
     </row>
     <row r="119" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="B119" t="s">
         <v>1</v>
@@ -4415,7 +4421,7 @@
     </row>
     <row r="123" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="B123" t="s">
         <v>1</v>
@@ -4423,7 +4429,7 @@
     </row>
     <row r="124" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="B124" t="s">
         <v>1</v>
@@ -4447,7 +4453,7 @@
     </row>
     <row r="127" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="B127" t="s">
         <v>1</v>
@@ -4471,7 +4477,7 @@
     </row>
     <row r="130" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="B130" t="s">
         <v>1</v>
@@ -4495,7 +4501,7 @@
     </row>
     <row r="133" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="B133" t="s">
         <v>1</v>
@@ -4511,7 +4517,7 @@
     </row>
     <row r="135" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="B135" t="s">
         <v>1</v>
@@ -4519,7 +4525,7 @@
     </row>
     <row r="136" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="B136" t="s">
         <v>1</v>
@@ -4527,7 +4533,7 @@
     </row>
     <row r="137" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="B137" t="s">
         <v>1</v>
@@ -4535,7 +4541,7 @@
     </row>
     <row r="138" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B138" t="s">
         <v>1</v>
@@ -4543,7 +4549,7 @@
     </row>
     <row r="139" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B139" t="s">
         <v>1</v>
@@ -4559,7 +4565,7 @@
     </row>
     <row r="141" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="B141" t="s">
         <v>1</v>
@@ -4607,7 +4613,7 @@
     </row>
     <row r="147" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="B147" t="s">
         <v>1</v>
@@ -4615,7 +4621,7 @@
     </row>
     <row r="148" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="B148" t="s">
         <v>1</v>
@@ -4655,7 +4661,7 @@
     </row>
     <row r="153" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="B153" t="s">
         <v>1</v>
@@ -4703,7 +4709,7 @@
     </row>
     <row r="159" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="B159" t="s">
         <v>1</v>
@@ -4711,7 +4717,7 @@
     </row>
     <row r="160" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="B160" t="s">
         <v>1</v>
@@ -4719,7 +4725,7 @@
     </row>
     <row r="161" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="B161" t="s">
         <v>1</v>
@@ -4735,7 +4741,7 @@
     </row>
     <row r="163" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="B163" t="s">
         <v>1</v>
@@ -4751,7 +4757,7 @@
     </row>
     <row r="165" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="B165" t="s">
         <v>1</v>
@@ -4759,7 +4765,7 @@
     </row>
     <row r="166" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B166" t="s">
         <v>1</v>
@@ -4767,7 +4773,7 @@
     </row>
     <row r="167" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="B167" t="s">
         <v>1</v>
@@ -4783,7 +4789,7 @@
     </row>
     <row r="169" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="B169" t="s">
         <v>1</v>
@@ -4791,7 +4797,7 @@
     </row>
     <row r="170" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="B170" t="s">
         <v>1</v>
@@ -4799,7 +4805,7 @@
     </row>
     <row r="171" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="B171" t="s">
         <v>1</v>
@@ -4831,7 +4837,7 @@
     </row>
     <row r="175" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="B175" t="s">
         <v>1</v>
@@ -4855,7 +4861,7 @@
     </row>
     <row r="178" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="B178" t="s">
         <v>1</v>
@@ -4863,7 +4869,7 @@
     </row>
     <row r="179" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="B179" t="s">
         <v>1</v>
@@ -4879,7 +4885,7 @@
     </row>
     <row r="181" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B181" t="s">
         <v>1</v>
@@ -4927,7 +4933,7 @@
     </row>
     <row r="187" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="B187" t="s">
         <v>1</v>
@@ -4943,7 +4949,7 @@
     </row>
     <row r="189" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="B189" t="s">
         <v>1</v>
@@ -4999,7 +5005,7 @@
     </row>
     <row r="196" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="B196" t="s">
         <v>1</v>
@@ -5031,7 +5037,7 @@
     </row>
     <row r="200" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="B200" t="s">
         <v>2</v>
@@ -5039,7 +5045,7 @@
     </row>
     <row r="201" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="B201" t="s">
         <v>2</v>
@@ -5047,7 +5053,7 @@
     </row>
     <row r="202" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="B202" t="s">
         <v>2</v>
@@ -5055,7 +5061,7 @@
     </row>
     <row r="203" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="B203" t="s">
         <v>2</v>
@@ -5063,7 +5069,7 @@
     </row>
     <row r="204" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="B204" t="s">
         <v>2</v>
@@ -5071,7 +5077,7 @@
     </row>
     <row r="205" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="B205" t="s">
         <v>2</v>
@@ -5079,7 +5085,7 @@
     </row>
     <row r="206" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="B206" t="s">
         <v>2</v>
@@ -5087,7 +5093,7 @@
     </row>
     <row r="207" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="B207" t="s">
         <v>2</v>
@@ -5095,7 +5101,7 @@
     </row>
     <row r="208" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="B208" t="s">
         <v>2</v>
@@ -5103,7 +5109,7 @@
     </row>
     <row r="209" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="B209" t="s">
         <v>2</v>
@@ -5111,7 +5117,7 @@
     </row>
     <row r="210" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="B210" t="s">
         <v>2</v>
@@ -5119,7 +5125,7 @@
     </row>
     <row r="211" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="B211" t="s">
         <v>2</v>
@@ -5127,7 +5133,7 @@
     </row>
     <row r="212" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="B212" t="s">
         <v>2</v>
@@ -5135,7 +5141,7 @@
     </row>
     <row r="213" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="B213" t="s">
         <v>2</v>
@@ -5143,7 +5149,7 @@
     </row>
     <row r="214" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="B214" t="s">
         <v>2</v>
@@ -5167,7 +5173,7 @@
     </row>
     <row r="217" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="B217" t="s">
         <v>2</v>
@@ -5175,7 +5181,7 @@
     </row>
     <row r="218" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="B218" t="s">
         <v>2</v>
@@ -5183,7 +5189,7 @@
     </row>
     <row r="219" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="B219" t="s">
         <v>2</v>
@@ -5191,7 +5197,7 @@
     </row>
     <row r="220" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="B220" t="s">
         <v>2</v>
@@ -5199,7 +5205,7 @@
     </row>
     <row r="221" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="B221" t="s">
         <v>2</v>
@@ -5207,7 +5213,7 @@
     </row>
     <row r="222" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="B222" t="s">
         <v>2</v>
@@ -5215,7 +5221,7 @@
     </row>
     <row r="223" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="B223" t="s">
         <v>2</v>
@@ -5223,7 +5229,7 @@
     </row>
     <row r="224" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="B224" t="s">
         <v>2</v>
@@ -5231,7 +5237,7 @@
     </row>
     <row r="225" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="B225" t="s">
         <v>2</v>
@@ -5239,7 +5245,7 @@
     </row>
     <row r="226" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="B226" t="s">
         <v>2</v>
@@ -5247,7 +5253,7 @@
     </row>
     <row r="227" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="B227" t="s">
         <v>2</v>
@@ -5255,7 +5261,7 @@
     </row>
     <row r="228" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="B228" t="s">
         <v>2</v>
@@ -5271,7 +5277,7 @@
     </row>
     <row r="230" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="B230" t="s">
         <v>2</v>
@@ -5279,7 +5285,7 @@
     </row>
     <row r="231" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="B231" t="s">
         <v>2</v>
@@ -5303,7 +5309,7 @@
     </row>
     <row r="234" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="B234" t="s">
         <v>2</v>
@@ -5311,7 +5317,7 @@
     </row>
     <row r="235" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="B235" t="s">
         <v>2</v>
@@ -5327,7 +5333,7 @@
     </row>
     <row r="237" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="B237" t="s">
         <v>2</v>
@@ -5335,7 +5341,7 @@
     </row>
     <row r="238" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="B238" t="s">
         <v>2</v>
@@ -5343,7 +5349,7 @@
     </row>
     <row r="239" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A239" s="1" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="B239" t="s">
         <v>2</v>
@@ -5359,7 +5365,7 @@
     </row>
     <row r="241" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="B241" t="s">
         <v>2</v>
@@ -5367,7 +5373,7 @@
     </row>
     <row r="242" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="B242" t="s">
         <v>2</v>
@@ -5407,7 +5413,7 @@
     </row>
     <row r="247" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="B247" t="s">
         <v>2</v>
@@ -5431,7 +5437,7 @@
     </row>
     <row r="250" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="B250" t="s">
         <v>2</v>
@@ -5439,7 +5445,7 @@
     </row>
     <row r="251" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="B251" t="s">
         <v>2</v>
@@ -5455,7 +5461,7 @@
     </row>
     <row r="253" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="B253" t="s">
         <v>2</v>
@@ -5487,7 +5493,7 @@
     </row>
     <row r="257" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="B257" t="s">
         <v>2</v>
@@ -5495,7 +5501,7 @@
     </row>
     <row r="258" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="B258" t="s">
         <v>2</v>
@@ -5503,7 +5509,7 @@
     </row>
     <row r="259" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="B259" t="s">
         <v>2</v>
@@ -5511,7 +5517,7 @@
     </row>
     <row r="260" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="B260" t="s">
         <v>2</v>
@@ -5519,7 +5525,7 @@
     </row>
     <row r="261" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="B261" t="s">
         <v>2</v>
@@ -5535,7 +5541,7 @@
     </row>
     <row r="263" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="B263" t="s">
         <v>2</v>
@@ -5543,7 +5549,7 @@
     </row>
     <row r="264" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="B264" t="s">
         <v>2</v>
@@ -5551,7 +5557,7 @@
     </row>
     <row r="265" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="B265" t="s">
         <v>2</v>
@@ -5559,7 +5565,7 @@
     </row>
     <row r="266" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="B266" t="s">
         <v>2</v>
@@ -5567,7 +5573,7 @@
     </row>
     <row r="267" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="B267" t="s">
         <v>2</v>
@@ -5575,7 +5581,7 @@
     </row>
     <row r="268" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="B268" t="s">
         <v>2</v>
@@ -5583,7 +5589,7 @@
     </row>
     <row r="269" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="B269" t="s">
         <v>2</v>
@@ -5591,7 +5597,7 @@
     </row>
     <row r="270" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="B270" t="s">
         <v>2</v>
@@ -5623,7 +5629,7 @@
     </row>
     <row r="274" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="B274" t="s">
         <v>2</v>
@@ -5631,7 +5637,7 @@
     </row>
     <row r="275" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="B275" t="s">
         <v>2</v>
@@ -5639,7 +5645,7 @@
     </row>
     <row r="276" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="B276" t="s">
         <v>2</v>
@@ -5647,7 +5653,7 @@
     </row>
     <row r="277" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="B277" t="s">
         <v>2</v>
@@ -5671,7 +5677,7 @@
     </row>
     <row r="280" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="B280" t="s">
         <v>2</v>
@@ -5679,7 +5685,7 @@
     </row>
     <row r="281" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="B281" t="s">
         <v>2</v>
@@ -5703,7 +5709,7 @@
     </row>
     <row r="284" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="B284" t="s">
         <v>2</v>
@@ -5727,7 +5733,7 @@
     </row>
     <row r="287" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="B287" t="s">
         <v>2</v>
@@ -5735,7 +5741,7 @@
     </row>
     <row r="288" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="B288" t="s">
         <v>2</v>
@@ -5751,7 +5757,7 @@
     </row>
     <row r="290" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="B290" t="s">
         <v>2</v>
@@ -5759,7 +5765,7 @@
     </row>
     <row r="291" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="B291" t="s">
         <v>2</v>
@@ -5767,7 +5773,7 @@
     </row>
     <row r="292" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="B292" t="s">
         <v>2</v>
@@ -5775,7 +5781,7 @@
     </row>
     <row r="293" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="B293" t="s">
         <v>2</v>
@@ -5791,7 +5797,7 @@
     </row>
     <row r="295" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="B295" t="s">
         <v>2</v>
@@ -5807,7 +5813,7 @@
     </row>
     <row r="297" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="B297" t="s">
         <v>2</v>
@@ -5823,7 +5829,7 @@
     </row>
     <row r="299" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="B299" t="s">
         <v>2</v>
@@ -5847,7 +5853,7 @@
     </row>
     <row r="302" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="B302" t="s">
         <v>2</v>
@@ -5855,7 +5861,7 @@
     </row>
     <row r="303" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="B303" t="s">
         <v>2</v>
@@ -5871,7 +5877,7 @@
     </row>
     <row r="305" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="B305" t="s">
         <v>2</v>
@@ -5879,7 +5885,7 @@
     </row>
     <row r="306" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="B306" t="s">
         <v>2</v>
@@ -5887,7 +5893,7 @@
     </row>
     <row r="307" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="B307" t="s">
         <v>2</v>
@@ -5927,7 +5933,7 @@
     </row>
     <row r="312" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="B312" t="s">
         <v>2</v>
@@ -5935,7 +5941,7 @@
     </row>
     <row r="313" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="B313" t="s">
         <v>2</v>
@@ -5975,7 +5981,7 @@
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="B318" t="s">
         <v>3</v>
@@ -5983,7 +5989,7 @@
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="B319" t="s">
         <v>3</v>
@@ -5991,7 +5997,7 @@
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="B320" t="s">
         <v>3</v>
@@ -6007,7 +6013,7 @@
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="B322" t="s">
         <v>3</v>
@@ -6015,7 +6021,7 @@
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="B323" t="s">
         <v>3</v>
@@ -6023,7 +6029,7 @@
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="B324" t="s">
         <v>3</v>
@@ -6031,7 +6037,7 @@
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A325" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="B325" t="s">
         <v>3</v>
@@ -6055,7 +6061,7 @@
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="B328" t="s">
         <v>3</v>
@@ -6063,7 +6069,7 @@
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A329" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="B329" t="s">
         <v>3</v>
@@ -6071,7 +6077,7 @@
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="B330" t="s">
         <v>3</v>
@@ -6087,7 +6093,7 @@
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A332" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="B332" t="s">
         <v>3</v>
@@ -6127,7 +6133,7 @@
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A337" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="B337" t="s">
         <v>3</v>
@@ -6135,7 +6141,7 @@
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A338" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="B338" t="s">
         <v>4</v>
@@ -6143,7 +6149,7 @@
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A339" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="B339" t="s">
         <v>4</v>
@@ -6151,7 +6157,7 @@
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A340" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="B340" t="s">
         <v>4</v>
@@ -6159,7 +6165,7 @@
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A341" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="B341" t="s">
         <v>4</v>
@@ -6167,7 +6173,7 @@
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A342" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="B342" t="s">
         <v>4</v>
@@ -6175,7 +6181,7 @@
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A343" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="B343" t="s">
         <v>4</v>
@@ -6183,7 +6189,7 @@
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A344" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="B344" t="s">
         <v>4</v>
@@ -6191,7 +6197,7 @@
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A345" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="B345" t="s">
         <v>4</v>
@@ -6215,7 +6221,7 @@
     </row>
     <row r="348" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A348" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="B348" t="s">
         <v>4</v>
@@ -6239,7 +6245,7 @@
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A351" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="B351" t="s">
         <v>4</v>
@@ -6247,7 +6253,7 @@
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A352" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="B352" t="s">
         <v>4</v>
@@ -6255,7 +6261,7 @@
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A353" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="B353" t="s">
         <v>4</v>
@@ -6279,7 +6285,7 @@
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A356" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="B356" t="s">
         <v>4</v>
@@ -6287,7 +6293,7 @@
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A357" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="B357" t="s">
         <v>4</v>
@@ -6295,7 +6301,7 @@
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A358" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="B358" t="s">
         <v>4</v>
@@ -6311,7 +6317,7 @@
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A360" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="B360" t="s">
         <v>4</v>
@@ -6319,7 +6325,7 @@
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A361" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="B361" t="s">
         <v>4</v>
@@ -6399,7 +6405,7 @@
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A371" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="B371" t="s">
         <v>152</v>
@@ -6407,7 +6413,7 @@
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A372" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="B372" t="s">
         <v>152</v>
@@ -6415,7 +6421,7 @@
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A373" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="B373" t="s">
         <v>152</v>
@@ -6439,7 +6445,7 @@
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A376" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="B376" t="s">
         <v>152</v>
@@ -6495,7 +6501,7 @@
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A383" s="3" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="B383" s="3" t="s">
         <v>154</v>
@@ -6599,7 +6605,7 @@
     </row>
     <row r="396" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A396" s="5" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="B396" t="s">
         <v>156</v>
@@ -6679,7 +6685,7 @@
     </row>
     <row r="406" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A406" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="B406" t="s">
         <v>156</v>
@@ -6719,7 +6725,7 @@
     </row>
     <row r="411" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A411" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="B411" t="s">
         <v>156</v>
@@ -6735,7 +6741,7 @@
     </row>
     <row r="413" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A413" s="5" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="B413" t="s">
         <v>156</v>
@@ -6871,7 +6877,7 @@
     </row>
     <row r="430" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A430" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="B430" t="s">
         <v>156</v>
@@ -6879,7 +6885,7 @@
     </row>
     <row r="431" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A431" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="B431" t="s">
         <v>158</v>
@@ -6887,7 +6893,7 @@
     </row>
     <row r="432" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A432" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="B432" t="s">
         <v>158</v>
@@ -6927,7 +6933,7 @@
     </row>
     <row r="437" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A437" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="B437" t="s">
         <v>158</v>
@@ -6935,7 +6941,7 @@
     </row>
     <row r="438" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A438" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="B438" t="s">
         <v>158</v>
@@ -6999,7 +7005,7 @@
     </row>
     <row r="446" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A446" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="B446" t="s">
         <v>158</v>
@@ -7047,7 +7053,7 @@
     </row>
     <row r="452" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A452" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="B452" t="s">
         <v>158</v>
@@ -7071,7 +7077,7 @@
     </row>
     <row r="455" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A455" s="1" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="B455" t="s">
         <v>158</v>
@@ -7079,7 +7085,7 @@
     </row>
     <row r="456" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A456" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="B456" t="s">
         <v>158</v>
@@ -7143,7 +7149,7 @@
     </row>
     <row r="464" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A464" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="B464" t="s">
         <v>158</v>
@@ -7159,7 +7165,7 @@
     </row>
     <row r="466" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A466" s="1" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="B466" t="s">
         <v>158</v>
@@ -7207,7 +7213,7 @@
     </row>
     <row r="472" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A472" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="B472" t="s">
         <v>158</v>
@@ -7231,7 +7237,7 @@
     </row>
     <row r="475" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A475" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="B475" t="s">
         <v>158</v>
@@ -7239,7 +7245,7 @@
     </row>
     <row r="476" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A476" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="B476" t="s">
         <v>158</v>
@@ -7255,7 +7261,7 @@
     </row>
     <row r="478" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A478" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="B478" t="s">
         <v>158</v>
@@ -7263,7 +7269,7 @@
     </row>
     <row r="479" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A479" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="B479" t="s">
         <v>158</v>
@@ -7271,7 +7277,7 @@
     </row>
     <row r="480" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A480" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="B480" t="s">
         <v>158</v>
@@ -7287,7 +7293,7 @@
     </row>
     <row r="482" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A482" s="1" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="B482" t="s">
         <v>158</v>
@@ -7295,7 +7301,7 @@
     </row>
     <row r="483" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A483" s="1" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="B483" t="s">
         <v>158</v>
@@ -7303,7 +7309,7 @@
     </row>
     <row r="484" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A484" s="5" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="B484" t="s">
         <v>158</v>
@@ -7511,7 +7517,7 @@
     </row>
     <row r="510" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A510" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="B510" t="s">
         <v>158</v>
@@ -7519,7 +7525,7 @@
     </row>
     <row r="511" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A511" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="B511" t="s">
         <v>158</v>
@@ -7527,7 +7533,7 @@
     </row>
     <row r="512" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A512" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="B512" t="s">
         <v>158</v>
@@ -7535,7 +7541,7 @@
     </row>
     <row r="513" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A513" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="B513" t="s">
         <v>158</v>
@@ -7543,7 +7549,7 @@
     </row>
     <row r="514" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A514" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="B514" t="s">
         <v>158</v>
@@ -7591,7 +7597,7 @@
     </row>
     <row r="520" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A520" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="B520" t="s">
         <v>160</v>
@@ -7607,7 +7613,7 @@
     </row>
     <row r="522" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A522" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="B522" t="s">
         <v>160</v>
@@ -7615,7 +7621,7 @@
     </row>
     <row r="523" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A523" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="B523" t="s">
         <v>160</v>
@@ -7623,7 +7629,7 @@
     </row>
     <row r="524" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A524" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="B524" t="s">
         <v>160</v>
@@ -7639,7 +7645,7 @@
     </row>
     <row r="526" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A526" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="B526" t="s">
         <v>160</v>
@@ -7647,7 +7653,7 @@
     </row>
     <row r="527" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A527" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="B527" t="s">
         <v>160</v>
@@ -7687,7 +7693,7 @@
     </row>
     <row r="532" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A532" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="B532" t="s">
         <v>160</v>
@@ -7695,7 +7701,7 @@
     </row>
     <row r="533" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A533" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="B533" t="s">
         <v>160</v>
@@ -7839,7 +7845,7 @@
     </row>
     <row r="551" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A551" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="B551" t="s">
         <v>160</v>
@@ -7871,7 +7877,7 @@
     </row>
     <row r="555" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A555" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="B555" t="s">
         <v>160</v>
@@ -7895,7 +7901,7 @@
     </row>
     <row r="558" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A558" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="B558" t="s">
         <v>162</v>
@@ -7919,7 +7925,7 @@
     </row>
     <row r="561" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A561" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="B561" t="s">
         <v>162</v>
@@ -7927,7 +7933,7 @@
     </row>
     <row r="562" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A562" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="B562" t="s">
         <v>162</v>
@@ -7935,7 +7941,7 @@
     </row>
     <row r="563" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A563" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="B563" t="s">
         <v>162</v>
@@ -7943,7 +7949,7 @@
     </row>
     <row r="564" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A564" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="B564" t="s">
         <v>162</v>
@@ -7967,7 +7973,7 @@
     </row>
     <row r="567" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A567" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="B567" t="s">
         <v>162</v>
@@ -7991,7 +7997,7 @@
     </row>
     <row r="570" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A570" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="B570" t="s">
         <v>162</v>
@@ -7999,7 +8005,7 @@
     </row>
     <row r="571" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A571" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="B571" t="s">
         <v>162</v>
@@ -8007,7 +8013,7 @@
     </row>
     <row r="572" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A572" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="B572" t="s">
         <v>162</v>
@@ -8023,7 +8029,7 @@
     </row>
     <row r="574" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A574" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="B574" t="s">
         <v>162</v>
@@ -8031,7 +8037,7 @@
     </row>
     <row r="575" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A575" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="B575" t="s">
         <v>162</v>
@@ -8039,7 +8045,7 @@
     </row>
     <row r="576" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A576" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="B576" t="s">
         <v>162</v>
@@ -8103,7 +8109,7 @@
     </row>
     <row r="584" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A584" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="B584" t="s">
         <v>162</v>
@@ -8119,7 +8125,7 @@
     </row>
     <row r="586" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A586" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="B586" t="s">
         <v>162</v>
@@ -8127,7 +8133,7 @@
     </row>
     <row r="587" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A587" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="B587" t="s">
         <v>162</v>
@@ -8135,7 +8141,7 @@
     </row>
     <row r="588" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A588" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="B588" t="s">
         <v>162</v>
@@ -8215,7 +8221,7 @@
     </row>
     <row r="598" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A598" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="B598" t="s">
         <v>162</v>
@@ -8223,7 +8229,7 @@
     </row>
     <row r="599" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A599" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="B599" t="s">
         <v>162</v>
@@ -8239,7 +8245,7 @@
     </row>
     <row r="601" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A601" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="B601" t="s">
         <v>162</v>
@@ -8247,7 +8253,7 @@
     </row>
     <row r="602" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A602" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="B602" t="s">
         <v>162</v>
@@ -8255,7 +8261,7 @@
     </row>
     <row r="603" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A603" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="B603" t="s">
         <v>162</v>
@@ -8279,7 +8285,7 @@
     </row>
     <row r="606" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A606" s="1" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="B606" t="s">
         <v>335</v>
@@ -8335,7 +8341,7 @@
     </row>
     <row r="613" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A613" s="1" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="B613" t="s">
         <v>335</v>
@@ -8543,7 +8549,7 @@
     </row>
     <row r="639" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A639" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="B639" t="s">
         <v>337</v>
@@ -8551,7 +8557,7 @@
     </row>
     <row r="640" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A640" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="B640" t="s">
         <v>337</v>
@@ -8591,7 +8597,7 @@
     </row>
     <row r="645" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A645" s="1" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="B645" t="s">
         <v>337</v>
@@ -8655,7 +8661,7 @@
     </row>
     <row r="653" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A653" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="B653" t="s">
         <v>337</v>
@@ -8687,7 +8693,7 @@
     </row>
     <row r="657" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A657" s="5" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="B657" t="s">
         <v>337</v>
@@ -8759,7 +8765,7 @@
     </row>
     <row r="666" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A666" s="1" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="B666" t="s">
         <v>337</v>
@@ -9023,7 +9029,7 @@
     </row>
     <row r="699" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A699" s="5" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="B699" t="s">
         <v>337</v>
@@ -9351,7 +9357,7 @@
     </row>
     <row r="740" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A740" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="B740" t="s">
         <v>337</v>
@@ -9359,7 +9365,7 @@
     </row>
     <row r="741" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A741" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B741" t="s">
         <v>337</v>
@@ -9367,7 +9373,7 @@
     </row>
     <row r="742" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A742" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="B742" t="s">
         <v>337</v>
@@ -9375,7 +9381,7 @@
     </row>
     <row r="743" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A743" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="B743" t="s">
         <v>337</v>
@@ -9383,7 +9389,7 @@
     </row>
     <row r="744" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A744" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="B744" t="s">
         <v>337</v>
@@ -9391,7 +9397,7 @@
     </row>
     <row r="745" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A745" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="B745" t="s">
         <v>337</v>
@@ -9399,7 +9405,7 @@
     </row>
     <row r="746" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A746" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="B746" t="s">
         <v>337</v>
@@ -9407,7 +9413,7 @@
     </row>
     <row r="747" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A747" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="B747" t="s">
         <v>338</v>
@@ -9415,7 +9421,7 @@
     </row>
     <row r="748" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A748" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="B748" t="s">
         <v>338</v>
@@ -9455,7 +9461,7 @@
     </row>
     <row r="753" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A753" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="B753" t="s">
         <v>338</v>
@@ -9487,7 +9493,7 @@
     </row>
     <row r="757" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A757" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="B757" t="s">
         <v>338</v>
@@ -9527,7 +9533,7 @@
     </row>
     <row r="762" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A762" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="B762" t="s">
         <v>338</v>
@@ -9551,7 +9557,7 @@
     </row>
     <row r="765" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A765" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="B765" t="s">
         <v>338</v>
@@ -9559,7 +9565,7 @@
     </row>
     <row r="766" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A766" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="B766" t="s">
         <v>338</v>
@@ -9655,31 +9661,31 @@
     </row>
     <row r="778" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A778" t="s">
-        <v>488</v>
+        <v>836</v>
       </c>
       <c r="B778" t="s">
         <v>340</v>
       </c>
     </row>
     <row r="779" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A779" s="4" t="s">
-        <v>489</v>
+      <c r="A779" t="s">
+        <v>837</v>
       </c>
       <c r="B779" t="s">
         <v>340</v>
       </c>
     </row>
     <row r="780" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A780" t="s">
-        <v>490</v>
+      <c r="A780" s="4" t="s">
+        <v>838</v>
       </c>
       <c r="B780" t="s">
         <v>340</v>
       </c>
     </row>
     <row r="781" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A781" t="s">
-        <v>492</v>
+      <c r="A781" s="4" t="s">
+        <v>839</v>
       </c>
       <c r="B781" t="s">
         <v>340</v>
@@ -9687,7 +9693,7 @@
     </row>
     <row r="782" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A782" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
       <c r="B782" t="s">
         <v>340</v>
@@ -9695,7 +9701,7 @@
     </row>
     <row r="783" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A783" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="B783" t="s">
         <v>340</v>
@@ -9703,7 +9709,7 @@
     </row>
     <row r="784" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A784" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="B784" t="s">
         <v>340</v>
@@ -9711,15 +9717,15 @@
     </row>
     <row r="785" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A785" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="B785" t="s">
         <v>340</v>
       </c>
     </row>
     <row r="786" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A786" s="5" t="s">
-        <v>497</v>
+      <c r="A786" t="s">
+        <v>493</v>
       </c>
       <c r="B786" t="s">
         <v>340</v>
@@ -9727,15 +9733,15 @@
     </row>
     <row r="787" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A787" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="B787" t="s">
         <v>340</v>
       </c>
     </row>
     <row r="788" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A788" t="s">
-        <v>499</v>
+      <c r="A788" s="5" t="s">
+        <v>495</v>
       </c>
       <c r="B788" t="s">
         <v>340</v>
@@ -9743,7 +9749,7 @@
     </row>
     <row r="789" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A789" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="B789" t="s">
         <v>340</v>
@@ -9751,7 +9757,7 @@
     </row>
     <row r="790" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A790" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="B790" t="s">
         <v>340</v>
@@ -9759,7 +9765,7 @@
     </row>
     <row r="791" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A791" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="B791" t="s">
         <v>340</v>
@@ -9767,7 +9773,7 @@
     </row>
     <row r="792" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A792" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="B792" t="s">
         <v>340</v>
@@ -9775,7 +9781,7 @@
     </row>
     <row r="793" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A793" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="B793" t="s">
         <v>340</v>
@@ -9783,15 +9789,15 @@
     </row>
     <row r="794" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A794" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="B794" t="s">
         <v>340</v>
       </c>
     </row>
     <row r="795" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A795" s="2" t="s">
-        <v>506</v>
+      <c r="A795" t="s">
+        <v>502</v>
       </c>
       <c r="B795" t="s">
         <v>340</v>
@@ -9799,15 +9805,15 @@
     </row>
     <row r="796" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A796" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="B796" t="s">
         <v>340</v>
       </c>
     </row>
     <row r="797" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A797" t="s">
-        <v>508</v>
+      <c r="A797" s="2" t="s">
+        <v>504</v>
       </c>
       <c r="B797" t="s">
         <v>340</v>
@@ -9815,7 +9821,7 @@
     </row>
     <row r="798" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A798" t="s">
-        <v>515</v>
+        <v>505</v>
       </c>
       <c r="B798" t="s">
         <v>340</v>
@@ -9823,7 +9829,7 @@
     </row>
     <row r="799" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A799" t="s">
-        <v>516</v>
+        <v>506</v>
       </c>
       <c r="B799" t="s">
         <v>340</v>
@@ -9831,7 +9837,7 @@
     </row>
     <row r="800" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A800" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="B800" t="s">
         <v>340</v>
@@ -9839,7 +9845,7 @@
     </row>
     <row r="801" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A801" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="B801" t="s">
         <v>340</v>
@@ -9847,7 +9853,7 @@
     </row>
     <row r="802" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A802" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="B802" t="s">
         <v>340</v>
@@ -9855,7 +9861,7 @@
     </row>
     <row r="803" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A803" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="B803" t="s">
         <v>340</v>
@@ -9863,7 +9869,7 @@
     </row>
     <row r="804" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A804" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="B804" t="s">
         <v>340</v>
@@ -9871,15 +9877,15 @@
     </row>
     <row r="805" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A805" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="B805" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="806" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A806" s="1" t="s">
-        <v>523</v>
+    <row r="806" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A806" t="s">
+        <v>519</v>
       </c>
       <c r="B806" t="s">
         <v>340</v>
@@ -9887,39 +9893,39 @@
     </row>
     <row r="807" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A807" t="s">
-        <v>546</v>
+        <v>520</v>
       </c>
       <c r="B807" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="808" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A808" t="s">
-        <v>547</v>
+    <row r="808" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A808" s="1" t="s">
+        <v>521</v>
       </c>
       <c r="B808" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="809" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A809" s="1" t="s">
-        <v>524</v>
+    <row r="809" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A809" t="s">
+        <v>544</v>
       </c>
       <c r="B809" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="810" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A810" s="1" t="s">
-        <v>525</v>
+        <v>340</v>
+      </c>
+    </row>
+    <row r="810" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A810" t="s">
+        <v>545</v>
       </c>
       <c r="B810" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="811" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A811" s="1" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="B811" t="s">
         <v>342</v>
@@ -9927,7 +9933,7 @@
     </row>
     <row r="812" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A812" s="1" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="B812" t="s">
         <v>342</v>
@@ -9935,7 +9941,7 @@
     </row>
     <row r="813" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A813" s="1" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="B813" t="s">
         <v>342</v>
@@ -9943,7 +9949,7 @@
     </row>
     <row r="814" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A814" s="1" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="B814" t="s">
         <v>342</v>
@@ -9951,7 +9957,7 @@
     </row>
     <row r="815" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A815" s="1" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="B815" t="s">
         <v>342</v>
@@ -9959,7 +9965,7 @@
     </row>
     <row r="816" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A816" s="1" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="B816" t="s">
         <v>342</v>
@@ -9967,7 +9973,7 @@
     </row>
     <row r="817" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A817" s="1" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="B817" t="s">
         <v>342</v>
@@ -9975,7 +9981,7 @@
     </row>
     <row r="818" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A818" s="1" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="B818" t="s">
         <v>342</v>
@@ -9983,7 +9989,7 @@
     </row>
     <row r="819" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A819" s="1" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="B819" t="s">
         <v>342</v>
@@ -9991,23 +9997,23 @@
     </row>
     <row r="820" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A820" s="1" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="B820" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="821" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A821" t="s">
-        <v>536</v>
+    <row r="821" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A821" s="1" t="s">
+        <v>532</v>
       </c>
       <c r="B821" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="822" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A822" t="s">
-        <v>537</v>
+    <row r="822" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A822" s="1" t="s">
+        <v>533</v>
       </c>
       <c r="B822" t="s">
         <v>342</v>
@@ -10015,7 +10021,7 @@
     </row>
     <row r="823" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A823" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="B823" t="s">
         <v>342</v>
@@ -10023,7 +10029,7 @@
     </row>
     <row r="824" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A824" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="B824" t="s">
         <v>342</v>
@@ -10031,23 +10037,23 @@
     </row>
     <row r="825" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A825" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="B825" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="826" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A826" s="7" t="s">
-        <v>541</v>
+    <row r="826" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A826" t="s">
+        <v>537</v>
       </c>
       <c r="B826" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="827" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A827" s="7" t="s">
-        <v>542</v>
+    <row r="827" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A827" t="s">
+        <v>538</v>
       </c>
       <c r="B827" t="s">
         <v>342</v>
@@ -10055,7 +10061,7 @@
     </row>
     <row r="828" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A828" s="7" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="B828" t="s">
         <v>342</v>
@@ -10063,15 +10069,31 @@
     </row>
     <row r="829" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A829" s="7" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="B829" t="s">
         <v>342</v>
       </c>
     </row>
+    <row r="830" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A830" s="7" t="s">
+        <v>541</v>
+      </c>
+      <c r="B830" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="831" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A831" s="7" t="s">
+        <v>542</v>
+      </c>
+      <c r="B831" t="s">
+        <v>342</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A25:B829">
-    <sortCondition ref="B25:B829"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A25:B831">
+    <sortCondition ref="B25:B831"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>